<commit_message>
resultados y analisis de no lienal
</commit_message>
<xml_diff>
--- a/codigo_final/final/Lineal_no_estacionario/resultados/resultados_finales.xlsx
+++ b/codigo_final/final/Lineal_no_estacionario/resultados/resultados_finales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pleal\Documents\Unal\Tesis\Codigo\Prediccion_Probabilistica\codigo_final\final\Lineal_no_estacionario\resultados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D071653-41AA-45B0-B458-7D42EE726971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DD38FF-17C6-4C11-9D82-3817343C8754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -499,7 +499,7 @@
   <dimension ref="A1:P841"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>